<commit_message>
investigated tree structure and added missingness analysis
</commit_message>
<xml_diff>
--- a/EDA Visualization.xlsx
+++ b/EDA Visualization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BensonIgarabuza\Documents\OMSA\ISYE6748\StiboSystems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE00B54-7254-4C28-B811-43D9BA527286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CC7DAA-80CA-4556-BA6A-C6EDE3B4CA3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A27755F7-EBC9-450D-BAD6-F899B717A89F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A27755F7-EBC9-450D-BAD6-F899B717A89F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Node</t>
   </si>
@@ -408,15 +408,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{806D00C9-5E3E-43AA-81AA-99010201ED1C}">
-  <dimension ref="C3:J13"/>
+  <dimension ref="C3:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -435,8 +435,20 @@
       <c r="J3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>7</v>
       </c>
@@ -455,8 +467,14 @@
       <c r="J4">
         <v>2833</v>
       </c>
-    </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>2833</v>
+      </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>21</v>
       </c>
@@ -475,8 +493,11 @@
       <c r="J5">
         <v>2833</v>
       </c>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>12</v>
       </c>
@@ -495,8 +516,11 @@
       <c r="J6">
         <v>2833</v>
       </c>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>21</v>
       </c>
@@ -515,8 +539,11 @@
       <c r="J7">
         <v>2833</v>
       </c>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>24</v>
       </c>
@@ -535,8 +562,11 @@
       <c r="J8">
         <v>2833</v>
       </c>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>25</v>
       </c>
@@ -552,8 +582,11 @@
       <c r="J9">
         <v>2833</v>
       </c>
-    </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>31</v>
       </c>
@@ -569,29 +602,46 @@
       <c r="J10">
         <v>2833</v>
       </c>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N10">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>32</v>
       </c>
       <c r="D11">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N11">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>47</v>
       </c>
       <c r="D12">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N12">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13">
         <v>2833</v>
+      </c>
+      <c r="N13">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="N14">
+        <v>2557</v>
       </c>
     </row>
   </sheetData>

</xml_diff>